<commit_message>
Added random seeds for repeatability
</commit_message>
<xml_diff>
--- a/Data/tables/main_event_attribute_info.xlsx
+++ b/Data/tables/main_event_attribute_info.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,12 +422,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Attribute</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
@@ -460,31 +448,31 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +484,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,19 +496,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,19 +520,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +544,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +556,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +580,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,19 +592,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,7 +616,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,19 +628,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,19 +652,19 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">

</xml_diff>